<commit_message>
Add more examples and perform analysis of the calculations
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hackvan/Desktop/resuelve_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85CC151-2111-9648-9CC0-8FA5B326D0A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AE70AA-A972-5C44-B861-95B76CCB2DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="960" windowWidth="24380" windowHeight="14500" xr2:uid="{86A960A6-9C1A-A441-9D82-1528B458BA70}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
   <si>
     <t>NIVEL</t>
   </si>
@@ -99,6 +99,69 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Equipo 1</t>
+  </si>
+  <si>
+    <t>rojo</t>
+  </si>
+  <si>
+    <t>Juan Perez</t>
+  </si>
+  <si>
+    <t>Equipo 2</t>
+  </si>
+  <si>
+    <t>azul</t>
+  </si>
+  <si>
+    <t>El Rulo</t>
+  </si>
+  <si>
+    <t>EL Cuauh</t>
+  </si>
+  <si>
+    <t>Cosme Fulanito</t>
+  </si>
+  <si>
+    <t>Etiquetas</t>
+  </si>
+  <si>
+    <t>Parametros</t>
+  </si>
+  <si>
+    <t>Entradas</t>
+  </si>
+  <si>
+    <t>Calculos Ind.</t>
+  </si>
+  <si>
+    <t>Calculos Grupo.</t>
+  </si>
+  <si>
+    <t>equipos</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>equipo1</t>
+  </si>
+  <si>
+    <t>total_goles</t>
+  </si>
+  <si>
+    <t>total_minimos</t>
+  </si>
+  <si>
+    <t>jugadores</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>equipo2</t>
   </si>
 </sst>
 </file>
@@ -133,12 +196,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -170,7 +257,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,14 +283,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency [0]" xfId="1" builtinId="7"/>
@@ -520,7 +634,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB7D9BB-E4A4-DC4E-9F58-7CDED34911B2}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -594,8 +708,10 @@
       <c r="O2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q2"/>
-      <c r="R2"/>
+      <c r="Q2" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="31"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
@@ -626,6 +742,10 @@
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="6"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
@@ -656,6 +776,10 @@
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="6"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
@@ -686,6 +810,10 @@
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="6"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
@@ -731,6 +859,10 @@
       <c r="O6" s="9">
         <f>J6+N6</f>
         <v>59550</v>
+      </c>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -758,97 +890,416 @@
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="17">
+        <v>0.5</v>
+      </c>
       <c r="I8" s="11"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="17">
+        <v>0.5</v>
+      </c>
       <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10"/>
-      <c r="B10"/>
       <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-    </row>
-    <row r="11" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11"/>
-      <c r="B11"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:18" s="12" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-      <c r="N11"/>
-      <c r="O11"/>
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12"/>
-      <c r="B12"/>
+      <c r="A12" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-      <c r="N12"/>
-      <c r="O12"/>
+      <c r="D12" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="20">
+        <v>10</v>
+      </c>
+      <c r="H12" s="16">
+        <f>VLOOKUP(F12,$A$3:$B$6,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="I12" s="22">
+        <f>G12/H12</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J12" s="23">
+        <v>50000</v>
+      </c>
+      <c r="K12" s="23">
+        <v>25000</v>
+      </c>
+      <c r="L12" s="24">
+        <f>(K12*$B$8)*I12</f>
+        <v>8333.3333333333321</v>
+      </c>
+      <c r="M12" s="24">
+        <f>(K12*$B$9)*$I$14</f>
+        <v>9500</v>
+      </c>
+      <c r="N12" s="24">
+        <f>IF(L12+M12&lt;=K12, L12+M12, K12)</f>
+        <v>17833.333333333332</v>
+      </c>
+      <c r="O12" s="25">
+        <f>J12+N12</f>
+        <v>67833.333333333328</v>
+      </c>
     </row>
     <row r="13" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="N13"/>
-      <c r="O13"/>
+      <c r="A13" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="20">
+        <v>9</v>
+      </c>
+      <c r="H13" s="16">
+        <f>VLOOKUP(F13,$A$3:$B$6,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="I13" s="22">
+        <f>G13/H13</f>
+        <v>0.9</v>
+      </c>
+      <c r="J13" s="23">
+        <v>30000</v>
+      </c>
+      <c r="K13" s="23">
+        <v>15000</v>
+      </c>
+      <c r="L13" s="24">
+        <f>(K13*$B$8)*I13</f>
+        <v>6750</v>
+      </c>
+      <c r="M13" s="24">
+        <f>(K13*$B$9)*$I$14</f>
+        <v>5700</v>
+      </c>
+      <c r="N13" s="24">
+        <f t="shared" ref="N13:N19" si="0">IF(L13+M13&lt;=K13, L13+M13, K13)</f>
+        <v>12450</v>
+      </c>
+      <c r="O13" s="25">
+        <f t="shared" ref="O13:O19" si="1">J13+N13</f>
+        <v>42450</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="G14" s="27">
+        <f>SUM(G12:G13)</f>
+        <v>19</v>
+      </c>
+      <c r="H14" s="27">
+        <f>SUM(H12:H13)</f>
+        <v>25</v>
+      </c>
+      <c r="I14" s="28">
+        <f>G14/H14</f>
+        <v>0.76</v>
+      </c>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="30"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I15" s="11"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="30"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+    </row>
+    <row r="17" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="D17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D18" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="20">
+        <v>30</v>
+      </c>
+      <c r="H18" s="16">
+        <f t="shared" ref="H18:H19" si="2">VLOOKUP(F18,$A$3:$B$6,2,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="I18" s="22">
+        <f>G18/H18</f>
+        <v>1.5</v>
+      </c>
+      <c r="J18" s="23">
+        <v>100000</v>
+      </c>
+      <c r="K18" s="23">
+        <v>30000</v>
+      </c>
+      <c r="L18" s="24">
+        <f>(K18*$B$8)*I18</f>
+        <v>22500</v>
+      </c>
+      <c r="M18" s="24">
+        <f>(K18*$B$9)*$I$20</f>
+        <v>22200</v>
+      </c>
+      <c r="N18" s="24">
+        <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
+      <c r="O18" s="25">
+        <f t="shared" si="1"/>
+        <v>130000</v>
+      </c>
     </row>
     <row r="19" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-      <c r="O19"/>
+      <c r="D19" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="20">
+        <v>7</v>
+      </c>
+      <c r="H19" s="16">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="I19" s="22">
+        <f>G19/H19</f>
+        <v>1.4</v>
+      </c>
+      <c r="J19" s="23">
+        <v>20000</v>
+      </c>
+      <c r="K19" s="23">
+        <v>10000</v>
+      </c>
+      <c r="L19" s="24">
+        <f>(K19*$B$8)*I19</f>
+        <v>7000</v>
+      </c>
+      <c r="M19" s="24">
+        <f>(K19*$B$9)*$I$20</f>
+        <v>7400</v>
+      </c>
+      <c r="N19" s="24">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="O19" s="25">
+        <f t="shared" si="1"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G20" s="27">
+        <f>SUM(G18:G19)</f>
+        <v>37</v>
+      </c>
+      <c r="H20" s="27">
+        <f>SUM(H18:H19)</f>
+        <v>25</v>
+      </c>
+      <c r="I20" s="28">
+        <f>G20/H20</f>
+        <v>1.48</v>
+      </c>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="30"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="Q2:R2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create Level class with specs blueprint
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hackvan/Desktop/resuelve_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AE70AA-A972-5C44-B861-95B76CCB2DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C890706-EEA4-3F42-83DF-6C633F62C983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="960" windowWidth="24380" windowHeight="14500" xr2:uid="{86A960A6-9C1A-A441-9D82-1528B458BA70}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
   <si>
     <t>NIVEL</t>
   </si>
@@ -162,15 +162,65 @@
   </si>
   <si>
     <t>equipo2</t>
+  </si>
+  <si>
+    <t>Class Team</t>
+  </si>
+  <si>
+    <t>Class Level</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>goals_for_months</t>
+  </si>
+  <si>
+    <t>goals_by_month</t>
+  </si>
+  <si>
+    <t>goals_by_levels</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>Class Player</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>goals_by_level</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>base_bonus</t>
+  </si>
+  <si>
+    <t>individual_bonus</t>
+  </si>
+  <si>
+    <t>team_bonus</t>
+  </si>
+  <si>
+    <t>total_payment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;COP&quot;* #,##0_);_(&quot;COP&quot;* \(#,##0\);_(&quot;COP&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -252,12 +302,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -313,13 +364,44 @@
     <xf numFmtId="10" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="1" builtinId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
@@ -634,9 +716,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB7D9BB-E4A4-DC4E-9F58-7CDED34911B2}">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -708,10 +792,10 @@
       <c r="O2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="31" t="s">
+      <c r="Q2" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="31"/>
+      <c r="R2" s="33"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
@@ -810,7 +894,7 @@
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="6"/>
-      <c r="Q5" s="32"/>
+      <c r="Q5" s="31"/>
       <c r="R5" s="6" t="s">
         <v>33</v>
       </c>
@@ -860,7 +944,7 @@
         <f>J6+N6</f>
         <v>59550</v>
       </c>
-      <c r="Q6" s="33"/>
+      <c r="Q6" s="32"/>
       <c r="R6" s="6" t="s">
         <v>34</v>
       </c>
@@ -1093,7 +1177,7 @@
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
     </row>
-    <row r="17" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="D17" s="3" t="s">
         <v>10</v>
       </c>
@@ -1131,7 +1215,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D18" s="20" t="s">
         <v>26</v>
       </c>
@@ -1175,7 +1259,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D19" s="20" t="s">
         <v>26</v>
       </c>
@@ -1219,7 +1303,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="G20" s="27">
         <f>SUM(G18:G19)</f>
         <v>37</v>
@@ -1239,41 +1323,84 @@
       <c r="N20" s="29"/>
       <c r="O20" s="30"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>35</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K23" t="s">
+        <v>43</v>
+      </c>
+      <c r="O23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>37</v>
       </c>
       <c r="C24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L24" t="s">
+        <v>45</v>
+      </c>
+      <c r="M24" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="P24" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q24" s="35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L25" t="s">
+        <v>46</v>
+      </c>
+      <c r="M25" s="36">
+        <v>19</v>
+      </c>
+      <c r="P25" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q25" s="35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L26" t="s">
+        <v>48</v>
+      </c>
+      <c r="M26" s="36">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>40</v>
       </c>
       <c r="E27" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L27" t="s">
+        <v>49</v>
+      </c>
+      <c r="M27" s="37">
+        <f>M25/M26</f>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>42</v>
       </c>
@@ -1281,19 +1408,111 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L30" t="s">
+        <v>45</v>
+      </c>
+      <c r="M30" s="38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>40</v>
+      </c>
+      <c r="L31" t="s">
+        <v>51</v>
+      </c>
+      <c r="M31" s="38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L32" t="s">
+        <v>52</v>
+      </c>
+      <c r="M32" s="38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>46</v>
+      </c>
+      <c r="M33" s="39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L34" t="s">
+        <v>53</v>
+      </c>
+      <c r="M34" s="40">
+        <f>VLOOKUP(M32,$A$3:$B$6, 2,FALSE)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L35" t="s">
+        <v>49</v>
+      </c>
+      <c r="M35" s="41">
+        <f>M33/M34</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="36" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L36" t="s">
+        <v>54</v>
+      </c>
+      <c r="M36" s="42">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="37" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L37" t="s">
+        <v>55</v>
+      </c>
+      <c r="M37" s="42">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="38" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L38" t="s">
+        <v>56</v>
+      </c>
+      <c r="M38" s="43">
+        <f>M37*B8*M35</f>
+        <v>6750</v>
+      </c>
+    </row>
+    <row r="39" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L39" t="s">
+        <v>57</v>
+      </c>
+      <c r="M39" s="43">
+        <f>M37*$B$9*M27</f>
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="40" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L40" t="s">
+        <v>58</v>
+      </c>
+      <c r="M40" s="43">
+        <f>M36+M38+M39</f>
+        <v>42450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>